<commit_message>
updated jar calls for OS compatibility
</commit_message>
<xml_diff>
--- a/db/queries/predicted/ASIS_20161108_HerpInv_Database-NATIVE-NATIVE-gpt-4o-queries-predicted.xlsx
+++ b/db/queries/predicted/ASIS_20161108_HerpInv_Database-NATIVE-NATIVE-gpt-4o-queries-predicted.xlsx
@@ -677,16 +677,24 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>SELECT LOCATIONID, COUNT(*) AS TurtleCount
-FROM TBLFIELDDATATURTLEMEASUREMENTS
-GROUP BY LOCATIONID</t>
+          <t>SELECT 
+    LOCATIONID, 
+    COUNT(*) AS NumberOfTurtlesMeasured
+FROM 
+    TBLFIELDDATATURTLEMEASUREMENTS
+GROUP BY 
+    LOCATIONID</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>SELECT LOCATIONID, COUNT(*) AS TurtleCount
-FROM TBLFIELDDATATURTLEMEASUREMENTS
-GROUP BY LOCATIONID</t>
+          <t>SELECT 
+    LOCATIONID, 
+    COUNT(*) AS NumberOfTurtlesMeasured
+FROM 
+    TBLFIELDDATATURTLEMEASUREMENTS
+GROUP BY 
+    LOCATIONID</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -1641,31 +1649,31 @@
       <c r="H12" t="inlineStr">
         <is>
           <t>SELECT 
-    tm.RECORDID AS TurtleMeasurementRecordID, 
-    tm.COMMENTS AS MeasurementComments
+    TMT.RECORDID AS TurtleMeasurementRecordID, 
+    TMT.COMMENTS AS MeasurementComments
 FROM 
-    TBLFIELDDATATURTLEMEASUREMENTS tm
+    TBLFIELDDATATURTLEMEASUREMENTS TMT
 JOIN 
-    TBLFIELDDATATURTLETRAPSURVEYS ts ON tm.EVENTID = ts.EVENTID AND tm.LOCATIONID = ts.LOCATIONID
+    TBLFIELDDATATURTLETRAPSURVEYS TTS ON TMT.EVENTID = TTS.EVENTID AND TMT.LOCATIONID = TTS.LOCATIONID
 WHERE 
-    tm.SPECIES_CODE = ts.SPECIES_CODE 
-    AND tm.NOTCH_CODE = ts.NOTCH_CODE 
-    AND tm.SEX &lt;&gt; ts.SEX</t>
+    TMT.SPECIES_CODE = TTS.SPECIES_CODE 
+    AND TMT.NOTCH_CODE = TTS.NOTCH_CODE 
+    AND TMT.SEX &lt;&gt; TTS.SEX</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
           <t>SELECT 
-    tm.RECORDID AS TurtleMeasurementRecordID, 
-    tm.COMMENTS AS MeasurementComments
+    TMT.RECORDID AS TurtleMeasurementRecordID, 
+    TMT.COMMENTS AS MeasurementComments
 FROM 
-    TBLFIELDDATATURTLEMEASUREMENTS tm
+    TBLFIELDDATATURTLEMEASUREMENTS TMT
 JOIN 
-    TBLFIELDDATATURTLETRAPSURVEYS ts ON tm.EVENTID = ts.EVENTID AND tm.LOCATIONID = ts.LOCATIONID
+    TBLFIELDDATATURTLETRAPSURVEYS TTS ON TMT.EVENTID = TTS.EVENTID AND TMT.LOCATIONID = TTS.LOCATIONID
 WHERE 
-    tm.SPECIES_CODE = ts.SPECIES_CODE 
-    AND tm.NOTCH_CODE = ts.NOTCH_CODE 
-    AND tm.SEX &lt;&gt; ts.SEX</t>
+    TMT.SPECIES_CODE = TTS.SPECIES_CODE 
+    AND TMT.NOTCH_CODE = TTS.NOTCH_CODE 
+    AND TMT.SEX &lt;&gt; TTS.SEX</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -2213,20 +2221,20 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>SELECT O.AGENCY/TITLE AS Agency, COUNT(T.RECORDID) AS TurtleMeasurementCount
-FROM TBLFIELDDATATURTLEMEASUREMENTS T
-JOIN TBLEVENTDATAHERPS E ON T.EVENTID = E.EVENTID
-JOIN OBSERVER_LU O ON E.OBSINITS = O.OBSINITS
-GROUP BY O.AGENCY/TITLE</t>
+          <t>SELECT o.[AGENCY/TITLE] AS Agency, COUNT(t.RECORDID) AS TurtleMeasurementCount
+FROM TBLFIELDDATATURTLEMEASUREMENTS t
+JOIN TBLEVENTDATAHERPS e ON t.EVENTID = e.EVENTID
+JOIN OBSERVER_LU o ON e.OBSINITS = o.OBSINITS
+GROUP BY o.[AGENCY/TITLE]</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>SELECT O.AGENCY/TITLE AS Agency, COUNT(T.RECORDID) AS TurtleMeasurementCount
-FROM TBLFIELDDATATURTLEMEASUREMENTS T
-JOIN TBLEVENTDATAHERPS E ON T.EVENTID = E.EVENTID
-JOIN OBSERVER_LU O ON E.OBSINITS = O.OBSINITS
-GROUP BY O.AGENCY/TITLE</t>
+          <t>SELECT o.[AGENCY/TITLE] AS Agency, COUNT(t.RECORDID) AS TurtleMeasurementCount
+FROM TBLFIELDDATATURTLEMEASUREMENTS t
+JOIN TBLEVENTDATAHERPS e ON t.EVENTID = e.EVENTID
+JOIN OBSERVER_LU o ON e.OBSINITS = o.OBSINITS
+GROUP BY o.[AGENCY/TITLE]</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -2438,8 +2446,7 @@
           <t>SELECT DISTINCT O.OBSINITS, O.FIRSTNAME, O.LASTNAME
 FROM OBSERVER_LU O
 JOIN TLINKOBSERVERS LO ON O.OBSINITS = LO.OBSINITS
-JOIN TBLEVENTDATAHERPS EDH ON LO.EVENTID = EDH.EVENTID
-JOIN TBLFIELDDATATURTLEMEASUREMENTS TTM ON EDH.EVENTID = TTM.EVENTID</t>
+JOIN TBLFIELDDATATURTLEMEASUREMENTS TM ON LO.EVENTID = TM.EVENTID</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -2447,8 +2454,7 @@
           <t>SELECT DISTINCT O.OBSINITS, O.FIRSTNAME, O.LASTNAME
 FROM OBSERVER_LU O
 JOIN TLINKOBSERVERS LO ON O.OBSINITS = LO.OBSINITS
-JOIN TBLEVENTDATAHERPS EDH ON LO.EVENTID = EDH.EVENTID
-JOIN TBLFIELDDATATURTLEMEASUREMENTS TTM ON EDH.EVENTID = TTM.EVENTID</t>
+JOIN TBLFIELDDATATURTLEMEASUREMENTS TM ON LO.EVENTID = TM.EVENTID</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -2770,7 +2776,7 @@
 FROM TBLFIELDDATAMINNOWTRAPSURVEYS MT
 JOIN TLUSTAGE S ON MT.STAGE = S.STAGE
 GROUP BY S.DESCRIPTION
-ORDER BY S.DESCRIPTION</t>
+ORDER BY MinnowCount DESC</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -2779,7 +2785,7 @@
 FROM TBLFIELDDATAMINNOWTRAPSURVEYS MT
 JOIN TLUSTAGE S ON MT.STAGE = S.STAGE
 GROUP BY S.DESCRIPTION
-ORDER BY S.DESCRIPTION</t>
+ORDER BY MinnowCount DESC</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -3300,8 +3306,8 @@
           <t>SELECT B.BEHAVIOR, COUNT(*) AS RecordCount
 FROM TBLFIELDDATASNAKEDATACOLLECTION SDC
 JOIN TLUBEHAVIOR B ON SDC.BEHAVIOR = B.BEHAVIOR
-JOIN TBLFIELDDATACOVERBOARD FDC ON SDC.EVENTID = FDC.EVENTID AND SDC.SNAKEID = FDC.SNAKEID
-WHERE FDC.TYPE = 'coverboard'
+JOIN TBLFIELDDATACOVERBOARD CB ON SDC.EVENTID = CB.EVENTID AND SDC.SNAKEID = CB.SNAKEID
+WHERE CB.TYPE = 'coverboard'
 GROUP BY B.BEHAVIOR</t>
         </is>
       </c>
@@ -3310,8 +3316,8 @@
           <t>SELECT B.BEHAVIOR, COUNT(*) AS RecordCount
 FROM TBLFIELDDATASNAKEDATACOLLECTION SDC
 JOIN TLUBEHAVIOR B ON SDC.BEHAVIOR = B.BEHAVIOR
-JOIN TBLFIELDDATACOVERBOARD FDC ON SDC.EVENTID = FDC.EVENTID AND SDC.SNAKEID = FDC.SNAKEID
-WHERE FDC.TYPE = 'coverboard'
+JOIN TBLFIELDDATACOVERBOARD CB ON SDC.EVENTID = CB.EVENTID AND SDC.SNAKEID = CB.SNAKEID
+WHERE CB.TYPE = 'coverboard'
 GROUP BY B.BEHAVIOR</t>
         </is>
       </c>
@@ -3523,16 +3529,16 @@
         <is>
           <t>SELECT 
     LP.POINTID, 
-    FDC.SNAKEID, 
-    FDC.[BOARD_</t>
+    FDCB.SNAKEID, 
+    FDCB.[BOARD_</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
           <t>SELECT 
     LP.POINTID, 
-    FDC.SNAKEID, 
-    FDC.[BOARD_</t>
+    FDCB.SNAKEID, 
+    FDCB.[BOARD_</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -3740,27 +3746,27 @@
       <c r="H31" t="inlineStr">
         <is>
           <t>SELECT 
-    EDH.WEATHER, 
-    COUNT(EDH.EVENTID) AS EventCount, 
-    AVG(EDH.AIRTEMP) AS AvgAirTemp, 
-    AVG(EDH.WATERTEMP) AS AvgWaterTemp
+    WEATHER, 
+    COUNT(EVENTID) AS EventCount, 
+    AVG(AIRTEMP) AS AvgAirTemp, 
+    AVG(WATERTEMP) AS AvgWaterTemp
 FROM 
-    TBLEVENTDATAHERPS AS EDH
+    TBLEVENTDATAHERPS
 GROUP BY 
-    EDH.WEATHER</t>
+    WEATHER</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
           <t>SELECT 
-    EDH.WEATHER, 
-    COUNT(EDH.EVENTID) AS EventCount, 
-    AVG(EDH.AIRTEMP) AS AvgAirTemp, 
-    AVG(EDH.WATERTEMP) AS AvgWaterTemp
+    WEATHER, 
+    COUNT(EVENTID) AS EventCount, 
+    AVG(AIRTEMP) AS AvgAirTemp, 
+    AVG(WATERTEMP) AS AvgWaterTemp
 FROM 
-    TBLEVENTDATAHERPS AS EDH
+    TBLEVENTDATAHERPS
 GROUP BY 
-    EDH.WEATHER</t>
+    WEATHER</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -3856,16 +3862,24 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>SELECT OBSINITS, AVG(AIRTEMP) AS AverageAirTemperature
-FROM TBLEVENTDATAHERPS
-GROUP BY OBSINITS</t>
+          <t>SELECT 
+    EDH.OBSINITS, 
+    AVG(EDH.AIRTEMP) AS AverageAirTemperature
+FROM 
+    TBLEVENTDATAHERPS AS EDH
+GROUP BY 
+    EDH.OBSINITS</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>SELECT OBSINITS, AVG(AIRTEMP) AS AverageAirTemperature
-FROM TBLEVENTDATAHERPS
-GROUP BY OBSINITS</t>
+          <t>SELECT 
+    EDH.OBSINITS, 
+    AVG(EDH.AIRTEMP) AS AverageAirTemperature
+FROM 
+    TBLEVENTDATAHERPS AS EDH
+GROUP BY 
+    EDH.OBSINITS</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -3965,7 +3979,7 @@
     EDH.WEATHER, 
     AVG(EDH.AIRTEMP) AS AverageAirTemperature
 FROM 
-    TBLEVENTDATAHERPS EDH
+    TBLEVENTDATAHERPS AS EDH
 GROUP BY 
     EDH.WEATHER</t>
         </is>
@@ -3976,7 +3990,7 @@
     EDH.WEATHER, 
     AVG(EDH.AIRTEMP) AS AverageAirTemperature
 FROM 
-    TBLEVENTDATAHERPS EDH
+    TBLEVENTDATAHERPS AS EDH
 GROUP BY 
     EDH.WEATHER</t>
         </is>

</xml_diff>